<commit_message>
Output of the latest version of the script
</commit_message>
<xml_diff>
--- a/RUS-charts.xlsx
+++ b/RUS-charts.xlsx
@@ -9,13 +9,15 @@
   <sheets>
     <sheet name="GDP-demand" sheetId="1" r:id="rId1"/>
     <sheet name="GDP-production" sheetId="2" r:id="rId2"/>
+    <sheet name="Inflation rate (%)" sheetId="3" r:id="rId3"/>
+    <sheet name="Current account balance (% of G" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -42,6 +44,12 @@
   </si>
   <si>
     <t>Services (contribution, pp)</t>
+  </si>
+  <si>
+    <t>Inflation rate (%)</t>
+  </si>
+  <si>
+    <t>Current account balance (% of GDP)</t>
   </si>
 </sst>
 </file>
@@ -643,4 +651,126 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+      <c r="B4">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2018</v>
+      </c>
+      <c r="B5">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2019</v>
+      </c>
+      <c r="B6">
+        <v>4.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2018</v>
+      </c>
+      <c r="B5">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2019</v>
+      </c>
+      <c r="B6">
+        <v>3.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix bugs for other countries
</commit_message>
<xml_diff>
--- a/RUS-charts.xlsx
+++ b/RUS-charts.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet name="GDP-demand" sheetId="1" r:id="rId1"/>
     <sheet name="GDP-production" sheetId="2" r:id="rId2"/>
-    <sheet name="Inflation rate (%)" sheetId="3" r:id="rId3"/>
-    <sheet name="Current account balance (% of G" sheetId="4" r:id="rId4"/>
+    <sheet name="Unemployment rate (%)" sheetId="3" r:id="rId3"/>
+    <sheet name="Inflation rate (%)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -46,10 +46,10 @@
     <t>Services (contribution, pp)</t>
   </si>
   <si>
+    <t>Unemployment rate (%)</t>
+  </si>
+  <si>
     <t>Inflation rate (%)</t>
-  </si>
-  <si>
-    <t>Current account balance (% of GDP)</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
         <v>2015</v>
       </c>
       <c r="B2">
-        <v>15.5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -682,7 +682,7 @@
         <v>2016</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -690,7 +690,7 @@
         <v>2017</v>
       </c>
       <c r="B4">
-        <v>3.7</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -698,7 +698,7 @@
         <v>2018</v>
       </c>
       <c r="B5">
-        <v>2.9</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -735,7 +735,7 @@
         <v>2015</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -743,7 +743,7 @@
         <v>2016</v>
       </c>
       <c r="B3">
-        <v>1.9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -751,7 +751,7 @@
         <v>2017</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -759,7 +759,7 @@
         <v>2018</v>
       </c>
       <c r="B5">
-        <v>6.9</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -767,7 +767,7 @@
         <v>2019</v>
       </c>
       <c r="B6">
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>